<commit_message>
Final Changes to InputOutput Tables as per Tester Class, previously provided values were having some errors
</commit_message>
<xml_diff>
--- a/Artifacts/InputOutputTable.xlsx
+++ b/Artifacts/InputOutputTable.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MS Study\CMPE 202 Software Systems Engineering[Prof. Paul Nguyen]\Team Project(Kanban)[CryptoUnpluggers]\CryptoUnpluggers\CMPE202-CSUnplugged-PeruvianFlipCoin\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MS Study\CMPE 202 Software Systems Engineering[Prof. Paul Nguyen]\Team Project(Kanban)[CryptoUnpluggers]\CryptoUnpluggers\CMPE202-CSUnplugged-PeruvianFlipCoin\Artifacts\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -115,7 +115,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -162,11 +162,44 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -177,6 +210,19 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -494,13 +540,13 @@
   <dimension ref="B3:H9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="3" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="7" t="s">
         <v>0</v>
       </c>
       <c r="C3" s="3" t="s">
@@ -520,8 +566,8 @@
       </c>
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B4" s="1"/>
-      <c r="C4" s="1"/>
+      <c r="B4" s="4"/>
+      <c r="C4" s="5"/>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
@@ -531,7 +577,7 @@
       <c r="B5" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="C5" s="5" t="s">
         <v>7</v>
       </c>
       <c r="D5" s="1" t="s">
@@ -549,17 +595,17 @@
     </row>
     <row r="6" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B6" s="1"/>
-      <c r="C6" s="1"/>
+      <c r="C6" s="5"/>
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
       <c r="G6" s="1"/>
     </row>
     <row r="7" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B7" t="s">
+      <c r="B7" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="C7" s="5" t="s">
         <v>7</v>
       </c>
       <c r="D7" s="1" t="s">
@@ -578,7 +624,7 @@
     </row>
     <row r="8" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B8" s="1"/>
-      <c r="C8" s="1"/>
+      <c r="C8" s="5"/>
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
@@ -588,7 +634,7 @@
       <c r="B9" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C9" s="2" t="s">
+      <c r="C9" s="6" t="s">
         <v>9</v>
       </c>
       <c r="D9" s="2" t="s">

</xml_diff>